<commit_message>
Updated video playback test cases.
</commit_message>
<xml_diff>
--- a/Youtube_Manual_Testing.xlsx
+++ b/Youtube_Manual_Testing.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29301"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="64" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8E8618C-BEAE-4CCC-ACFF-BDD854B8B107}"/>
+  <xr:revisionPtr revIDLastSave="107" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5FBA82F-33F3-4465-A0FC-75659BA3EDD1}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="168">
   <si>
     <t>Kevin Garry
 9/9/2025</t>
@@ -66,85 +66,98 @@
     <t>TC01</t>
   </si>
   <si>
-    <t>Play a video</t>
-  </si>
-  <si>
-    <t>Click play on a video thumbnail</t>
-  </si>
-  <si>
-    <t>Video plays smoothly</t>
+    <t>User clicks play on a video.</t>
+  </si>
+  <si>
+    <t>1. Navigate to a video
+2. Click the play button</t>
+  </si>
+  <si>
+    <t>Video is played smoothly.</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
   <si>
     <t>TC02</t>
   </si>
   <si>
-    <t>Pause/Resume</t>
-  </si>
-  <si>
-    <t>Pause video during playback</t>
-  </si>
-  <si>
-    <t>Video pauses, resumes from same timestamp</t>
+    <t>User clicks the pause button on a video. User then resumes the video.</t>
+  </si>
+  <si>
+    <t>1. Navigate to a video
+2. Click the play button
+3. Click the pause button
+4. Click the play button again</t>
+  </si>
+  <si>
+    <t>Video is paused. Resumes from the same timestamp it was paused.</t>
   </si>
   <si>
     <t>TC03</t>
   </si>
   <si>
-    <t>Seek video</t>
-  </si>
-  <si>
-    <t>Drag seek bar to start/middle/end</t>
-  </si>
-  <si>
-    <t>Video jumps to correct point</t>
+    <t>User drags the seek bar to a specific point in a video.</t>
+  </si>
+  <si>
+    <t>1. Navigate to a video
+2. Click and hold the drag bar and drag it to desired time stamp</t>
+  </si>
+  <si>
+    <t>Video plays smoothly from the correct time stamp.</t>
   </si>
   <si>
     <t>TC04</t>
   </si>
   <si>
-    <t>Fullscreen toggle</t>
-  </si>
-  <si>
-    <t>Click fullscreen button</t>
-  </si>
-  <si>
-    <t>Video enters fullscreen; exits on ESC</t>
+    <t>User clicks the fullscreen button on a video.</t>
+  </si>
+  <si>
+    <t>1. Navigate to a video
+2. Press the full screen button</t>
+  </si>
+  <si>
+    <t>The video enters full screen mode. Exits full screen mode using ESC key.</t>
   </si>
   <si>
     <t>TC05</t>
   </si>
   <si>
-    <t>Adjust volume</t>
-  </si>
-  <si>
-    <t>Change volume slider</t>
-  </si>
-  <si>
-    <t>Audio changes correctly</t>
+    <t>User adjusts the volume.</t>
+  </si>
+  <si>
+    <t>1. Navigate to a video.
+2. Click and drag the audio to desired level</t>
+  </si>
+  <si>
+    <t>Audio is changed accordingly.</t>
   </si>
   <si>
     <t>TC06</t>
   </si>
   <si>
-    <t>Auto-play next video</t>
-  </si>
-  <si>
-    <t>Finish one video</t>
-  </si>
-  <si>
-    <t>Next video auto-plays</t>
+    <t>User auto-plays a video.</t>
+  </si>
+  <si>
+    <t>1. Navigate to a video
+2. Finish the video
+3. Let the next video auto-play</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The next video starts playing automatically. </t>
   </si>
   <si>
     <t>TC07</t>
   </si>
   <si>
-    <t>Closed captions</t>
-  </si>
-  <si>
-    <t>Enable captions</t>
-  </si>
-  <si>
-    <t>Captions appear synced</t>
+    <t>User enables closed captioning.</t>
+  </si>
+  <si>
+    <t>1. Navigate to a video
+2. Click on the CC button</t>
+  </si>
+  <si>
+    <t>Captions appear on the screen.</t>
   </si>
   <si>
     <t>User Interactions</t>
@@ -959,13 +972,13 @@
   <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
     <col min="3" max="3" width="35" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.5703125" bestFit="1" customWidth="1"/>
@@ -1017,114 +1030,128 @@
       <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" ht="38.25" customHeight="1">
+    <row r="5" spans="1:6" ht="69" customHeight="1">
       <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" ht="38.25" customHeight="1">
+    <row r="6" spans="1:6" ht="54.75" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="D6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" ht="38.25" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="C7" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="D7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" ht="38.25" customHeight="1">
+    <row r="8" spans="1:6" ht="50.25" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="C8" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="D8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" ht="38.25" customHeight="1">
+    <row r="9" spans="1:6" ht="54" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="C9" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="D9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" ht="38.25" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="C10" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="D10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="1"/>
+        <v>37</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" ht="33.75" customHeight="1">
       <c r="A11" s="10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="1"/>
@@ -1134,135 +1161,135 @@
     </row>
     <row r="12" spans="1:6" ht="66" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" ht="66" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" ht="66" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" ht="66" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" ht="66" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" ht="66" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" ht="66" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" ht="66" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" ht="28.5" customHeight="1">
       <c r="A20" s="10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1272,103 +1299,103 @@
     </row>
     <row r="21" spans="1:6" ht="51" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" ht="51" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" ht="51" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" ht="51" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" ht="51" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" ht="51" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" ht="48.75" customHeight="1">
       <c r="A27" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B27" s="11"/>
       <c r="C27" s="10"/>
@@ -1378,135 +1405,135 @@
     </row>
     <row r="28" spans="1:6" ht="63" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6" ht="63" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" ht="63" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" ht="63" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" ht="63" customHeight="1">
       <c r="A32" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:6" ht="63" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:6" ht="63" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
     </row>
     <row r="35" spans="1:6" ht="63" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
     </row>
     <row r="36" spans="1:6" ht="42" customHeight="1">
       <c r="A36" s="11" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B36" s="11"/>
       <c r="C36" s="10"/>
@@ -1516,87 +1543,87 @@
     </row>
     <row r="37" spans="1:6" ht="56.25" customHeight="1">
       <c r="A37" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
     </row>
     <row r="38" spans="1:6" ht="56.25" customHeight="1">
       <c r="A38" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
     </row>
     <row r="39" spans="1:6" ht="56.25" customHeight="1">
       <c r="A39" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
     </row>
     <row r="40" spans="1:6" ht="56.25" customHeight="1">
       <c r="A40" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="1:6" ht="56.25" customHeight="1">
       <c r="A41" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
     </row>
     <row r="42" spans="1:6" ht="29.25" customHeight="1">
       <c r="A42" s="10" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B42" s="11"/>
       <c r="C42" s="10"/>
@@ -1606,80 +1633,80 @@
     </row>
     <row r="43" spans="1:6" ht="59.25" customHeight="1">
       <c r="A43" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
     </row>
     <row r="44" spans="1:6" ht="59.25" customHeight="1">
       <c r="A44" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
     </row>
     <row r="45" spans="1:6" ht="59.25" customHeight="1">
       <c r="A45" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
     </row>
     <row r="46" spans="1:6" ht="59.25" customHeight="1">
       <c r="A46" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
     </row>
     <row r="47" spans="1:6" ht="59.25" customHeight="1">
       <c r="A47" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>

</xml_diff>

<commit_message>
Updated user interaction test cases.
</commit_message>
<xml_diff>
--- a/Youtube_Manual_Testing.xlsx
+++ b/Youtube_Manual_Testing.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29301"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="107" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5FBA82F-33F3-4465-A0FC-75659BA3EDD1}"/>
+  <xr:revisionPtr revIDLastSave="198" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{516EAA65-10BF-457A-A4EE-89DC1F55D552}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="178">
   <si>
     <t>Kevin Garry
 9/9/2025</t>
@@ -166,316 +166,372 @@
     <t>TC08</t>
   </si>
   <si>
-    <t>Like/Dislike video</t>
-  </si>
-  <si>
-    <t>Click like/dislike</t>
-  </si>
-  <si>
-    <t>Count updates correctly</t>
+    <t>User clicks the like button on a video.</t>
+  </si>
+  <si>
+    <t>1. Navigate to a video
+2. Click the like button</t>
+  </si>
+  <si>
+    <t>Like count increases properly.</t>
   </si>
   <si>
     <t>TC09</t>
   </si>
   <si>
+    <t>User clicks the dislike button on a video.</t>
+  </si>
+  <si>
+    <t>1. Navigate to a video
+2. Click the dislike button</t>
+  </si>
+  <si>
+    <t>Dislike count increases correctly.</t>
+  </si>
+  <si>
+    <t>TC10</t>
+  </si>
+  <si>
+    <t>User posts a comment on a video.</t>
+  </si>
+  <si>
+    <t>1. Navigate to a video
+2. Click add a comment
+3. Enter valid text
+4. Click the Comment button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comment is displayed under the video in the comments section. </t>
+  </si>
+  <si>
+    <t>TC11</t>
+  </si>
+  <si>
+    <t>User replies to another user's comment on a video.</t>
+  </si>
+  <si>
+    <t>1. Navigate to a video
+2. Navigate to a comment in the comments section
+3. Click the reply button
+4. Enter valid text
+5. Click the reply button</t>
+  </si>
+  <si>
+    <t>Comment is displayed properly under the video and nested under the original comment.</t>
+  </si>
+  <si>
+    <t>TC12</t>
+  </si>
+  <si>
+    <t>User subscribes to another user's channel.</t>
+  </si>
+  <si>
+    <t>1. Navigate to another user's channel
+2. Click the Subscribe button</t>
+  </si>
+  <si>
+    <t>Subscribe button is changed to a Subscribed button. Subscriber count is increased.</t>
+  </si>
+  <si>
+    <t>TC13</t>
+  </si>
+  <si>
+    <t>User unsubscribes from another user's channel.</t>
+  </si>
+  <si>
+    <t>1. Navigate to another user's channel
+2. Click the Subscribed button
+3. Click the Unsubscribe button</t>
+  </si>
+  <si>
+    <t>Subscribed button is changed to a Subscribe button. Subscriber count is decreased.</t>
+  </si>
+  <si>
+    <t>TC14</t>
+  </si>
+  <si>
+    <t>User shares a video.</t>
+  </si>
+  <si>
+    <t>1. Navigate to a video
+2. Click the share button
+3. Select preferred way to share</t>
+  </si>
+  <si>
+    <t>User is able to properly share the link to the video via mutliple different options.</t>
+  </si>
+  <si>
+    <t>TC15</t>
+  </si>
+  <si>
+    <t>User reports a video.</t>
+  </si>
+  <si>
+    <t>1. Navigate to a video
+2. Click the "..." button
+3. Click the Report button
+4. Select reason for report
+5. Click the Next button
+6. Click the Report button</t>
+  </si>
+  <si>
+    <t>User gets a confimation message "Thanks for helping our community".</t>
+  </si>
+  <si>
+    <t>TC16</t>
+  </si>
+  <si>
+    <t>User saves a video to a playlist.</t>
+  </si>
+  <si>
+    <t>1. Navigate to a video
+2. Click the "..." button
+3. Click the Save button
+4. Select which playlist to save the video to</t>
+  </si>
+  <si>
+    <t>Video is saved successfully and shows up in the playlist.</t>
+  </si>
+  <si>
+    <t>TC17</t>
+  </si>
+  <si>
+    <t>Notification on new video</t>
+  </si>
+  <si>
+    <t>1. Navigate to another user's channel
+2. Click the subscribe button
+3. Click the subscribed button
+4. Select All
+5. Wait for that User to upload a video</t>
+  </si>
+  <si>
+    <t>User gets a notification that a channel they are subscribed to has posted a new video.</t>
+  </si>
+  <si>
+    <t>Search &amp; Navigation</t>
+  </si>
+  <si>
+    <t>TC18</t>
+  </si>
+  <si>
+    <t>Search video</t>
+  </si>
+  <si>
+    <t>Enter keyword</t>
+  </si>
+  <si>
+    <t>Relevant results displayed</t>
+  </si>
+  <si>
+    <t>TC19</t>
+  </si>
+  <si>
+    <t>Search filters</t>
+  </si>
+  <si>
+    <t>Apply filters (date, duration)</t>
+  </si>
+  <si>
+    <t>Results update correctly</t>
+  </si>
+  <si>
+    <t>TC20</t>
+  </si>
+  <si>
+    <t>Trending tab</t>
+  </si>
+  <si>
+    <t>Click trending</t>
+  </si>
+  <si>
+    <t>Trending videos displayed</t>
+  </si>
+  <si>
+    <t>TC21</t>
+  </si>
+  <si>
+    <t>Category navigation</t>
+  </si>
+  <si>
+    <t>Click music, gaming, news</t>
+  </si>
+  <si>
+    <t>Videos update correctly</t>
+  </si>
+  <si>
+    <t>TC22</t>
+  </si>
+  <si>
+    <t>Video suggestions</t>
+  </si>
+  <si>
+    <t>Play video</t>
+  </si>
+  <si>
+    <t>Related videos suggested</t>
+  </si>
+  <si>
+    <t>TC23</t>
+  </si>
+  <si>
+    <t>Pagination/load more</t>
+  </si>
+  <si>
+    <t>Scroll or click next</t>
+  </si>
+  <si>
+    <t>More videos load</t>
+  </si>
+  <si>
+    <t>Upload &amp; Account Features</t>
+  </si>
+  <si>
+    <t>TC24</t>
+  </si>
+  <si>
+    <t>Upload video</t>
+  </si>
+  <si>
+    <t>Upload valid file</t>
+  </si>
+  <si>
+    <t>Video processes &amp; publishes</t>
+  </si>
+  <si>
+    <t>TC25</t>
+  </si>
+  <si>
+    <t>Edit video details</t>
+  </si>
+  <si>
+    <t>Change title/description</t>
+  </si>
+  <si>
+    <t>Changes saved correctly</t>
+  </si>
+  <si>
+    <t>TC26</t>
+  </si>
+  <si>
+    <t>Private/Public</t>
+  </si>
+  <si>
+    <t>Set visibility</t>
+  </si>
+  <si>
+    <t>Video visibility updates</t>
+  </si>
+  <si>
+    <t>TC27</t>
+  </si>
+  <si>
+    <t>Delete video</t>
+  </si>
+  <si>
+    <t>Delete uploaded video</t>
+  </si>
+  <si>
+    <t>Video removed from account</t>
+  </si>
+  <si>
+    <t>TC28</t>
+  </si>
+  <si>
+    <t>Video thumbnail</t>
+  </si>
+  <si>
+    <t>Change thumbnail</t>
+  </si>
+  <si>
+    <t>Thumbnail updates correctly</t>
+  </si>
+  <si>
+    <t>TC29</t>
+  </si>
+  <si>
+    <t>View history</t>
+  </si>
+  <si>
+    <t>Play videos</t>
+  </si>
+  <si>
+    <t>History records played videos</t>
+  </si>
+  <si>
+    <t>TC30</t>
+  </si>
+  <si>
+    <t>Liked videos</t>
+  </si>
+  <si>
+    <t>Like video</t>
+  </si>
+  <si>
+    <t>Appears in liked list</t>
+  </si>
+  <si>
+    <t>TC31</t>
+  </si>
+  <si>
+    <t>Watch later</t>
+  </si>
+  <si>
+    <t>Add video</t>
+  </si>
+  <si>
+    <t>Appears in “Watch Later”</t>
+  </si>
+  <si>
+    <t>Mobile / Responsiveness</t>
+  </si>
+  <si>
+    <t>TC32</t>
+  </si>
+  <si>
+    <t>Mobile playback</t>
+  </si>
+  <si>
+    <t>Play video on mobile</t>
+  </si>
+  <si>
+    <t>Plays correctly with responsive layout</t>
+  </si>
+  <si>
+    <t>TC33</t>
+  </si>
+  <si>
+    <t>Mobile commenting</t>
+  </si>
+  <si>
     <t>Add comment</t>
   </si>
   <si>
-    <t>Submit comment</t>
-  </si>
-  <si>
-    <t>Comment appears below video</t>
-  </si>
-  <si>
-    <t>TC10</t>
-  </si>
-  <si>
-    <t>Reply to comment</t>
-  </si>
-  <si>
-    <t>Reply to a comment</t>
-  </si>
-  <si>
-    <t>Nested comment displays correctly</t>
-  </si>
-  <si>
-    <t>TC11</t>
-  </si>
-  <si>
-    <t>Subscribe/Unsubscribe</t>
-  </si>
-  <si>
-    <t>Click subscribe button</t>
-  </si>
-  <si>
-    <t>Subscription count updates</t>
-  </si>
-  <si>
-    <t>TC12</t>
-  </si>
-  <si>
-    <t>Share video</t>
-  </si>
-  <si>
-    <t>Click share button</t>
-  </si>
-  <si>
-    <t>Copy link or share options appear</t>
-  </si>
-  <si>
-    <t>TC13</t>
-  </si>
-  <si>
-    <t>Report video</t>
-  </si>
-  <si>
-    <t>Flag inappropriate content</t>
-  </si>
-  <si>
-    <t>Confirmation message appears</t>
-  </si>
-  <si>
-    <t>TC14</t>
-  </si>
-  <si>
-    <t>Save to playlist</t>
-  </si>
-  <si>
-    <t>Add video to playlist</t>
-  </si>
-  <si>
-    <t>Video appears in playlist</t>
-  </si>
-  <si>
-    <t>TC15</t>
-  </si>
-  <si>
-    <t>Notification on new video</t>
-  </si>
-  <si>
-    <t>Subscribe → new video uploaded</t>
+    <t>Appears properly</t>
+  </si>
+  <si>
+    <t>TC34</t>
+  </si>
+  <si>
+    <t>Mobile search</t>
+  </si>
+  <si>
+    <t>Results display correctly</t>
+  </si>
+  <si>
+    <t>TC35</t>
+  </si>
+  <si>
+    <t>Mobile notifications</t>
+  </si>
+  <si>
+    <t>Subscribe → new video</t>
   </si>
   <si>
     <t>Notification appears</t>
   </si>
   <si>
-    <t>Search &amp; Navigation</t>
-  </si>
-  <si>
-    <t>TC16</t>
-  </si>
-  <si>
-    <t>Search video</t>
-  </si>
-  <si>
-    <t>Enter keyword</t>
-  </si>
-  <si>
-    <t>Relevant results displayed</t>
-  </si>
-  <si>
-    <t>TC17</t>
-  </si>
-  <si>
-    <t>Search filters</t>
-  </si>
-  <si>
-    <t>Apply filters (date, duration)</t>
-  </si>
-  <si>
-    <t>Results update correctly</t>
-  </si>
-  <si>
-    <t>TC18</t>
-  </si>
-  <si>
-    <t>Trending tab</t>
-  </si>
-  <si>
-    <t>Click trending</t>
-  </si>
-  <si>
-    <t>Trending videos displayed</t>
-  </si>
-  <si>
-    <t>TC19</t>
-  </si>
-  <si>
-    <t>Category navigation</t>
-  </si>
-  <si>
-    <t>Click music, gaming, news</t>
-  </si>
-  <si>
-    <t>Videos update correctly</t>
-  </si>
-  <si>
-    <t>TC20</t>
-  </si>
-  <si>
-    <t>Video suggestions</t>
-  </si>
-  <si>
-    <t>Play video</t>
-  </si>
-  <si>
-    <t>Related videos suggested</t>
-  </si>
-  <si>
-    <t>TC21</t>
-  </si>
-  <si>
-    <t>Pagination/load more</t>
-  </si>
-  <si>
-    <t>Scroll or click next</t>
-  </si>
-  <si>
-    <t>More videos load</t>
-  </si>
-  <si>
-    <t>Upload &amp; Account Features</t>
-  </si>
-  <si>
-    <t>TC22</t>
-  </si>
-  <si>
-    <t>Upload video</t>
-  </si>
-  <si>
-    <t>Upload valid file</t>
-  </si>
-  <si>
-    <t>Video processes &amp; publishes</t>
-  </si>
-  <si>
-    <t>TC23</t>
-  </si>
-  <si>
-    <t>Edit video details</t>
-  </si>
-  <si>
-    <t>Change title/description</t>
-  </si>
-  <si>
-    <t>Changes saved correctly</t>
-  </si>
-  <si>
-    <t>TC24</t>
-  </si>
-  <si>
-    <t>Private/Public</t>
-  </si>
-  <si>
-    <t>Set visibility</t>
-  </si>
-  <si>
-    <t>Video visibility updates</t>
-  </si>
-  <si>
-    <t>TC25</t>
-  </si>
-  <si>
-    <t>Delete video</t>
-  </si>
-  <si>
-    <t>Delete uploaded video</t>
-  </si>
-  <si>
-    <t>Video removed from account</t>
-  </si>
-  <si>
-    <t>TC26</t>
-  </si>
-  <si>
-    <t>Video thumbnail</t>
-  </si>
-  <si>
-    <t>Change thumbnail</t>
-  </si>
-  <si>
-    <t>Thumbnail updates correctly</t>
-  </si>
-  <si>
-    <t>TC27</t>
-  </si>
-  <si>
-    <t>View history</t>
-  </si>
-  <si>
-    <t>Play videos</t>
-  </si>
-  <si>
-    <t>History records played videos</t>
-  </si>
-  <si>
-    <t>TC28</t>
-  </si>
-  <si>
-    <t>Liked videos</t>
-  </si>
-  <si>
-    <t>Like video</t>
-  </si>
-  <si>
-    <t>Appears in liked list</t>
-  </si>
-  <si>
-    <t>TC29</t>
-  </si>
-  <si>
-    <t>Watch later</t>
-  </si>
-  <si>
-    <t>Add video</t>
-  </si>
-  <si>
-    <t>Appears in “Watch Later”</t>
-  </si>
-  <si>
-    <t>Mobile / Responsiveness</t>
-  </si>
-  <si>
-    <t>TC30</t>
-  </si>
-  <si>
-    <t>Mobile playback</t>
-  </si>
-  <si>
-    <t>Play video on mobile</t>
-  </si>
-  <si>
-    <t>Plays correctly with responsive layout</t>
-  </si>
-  <si>
-    <t>TC31</t>
-  </si>
-  <si>
-    <t>Mobile commenting</t>
-  </si>
-  <si>
-    <t>Appears properly</t>
-  </si>
-  <si>
-    <t>TC32</t>
-  </si>
-  <si>
-    <t>Mobile search</t>
-  </si>
-  <si>
-    <t>Results display correctly</t>
-  </si>
-  <si>
-    <t>TC33</t>
-  </si>
-  <si>
-    <t>Mobile notifications</t>
-  </si>
-  <si>
-    <t>Subscribe → new video</t>
-  </si>
-  <si>
-    <t>TC34</t>
+    <t>TC36</t>
   </si>
   <si>
     <t>Mobile fullscreen</t>
@@ -490,7 +546,7 @@
     <t>Edge Cases / Exploratory</t>
   </si>
   <si>
-    <t>TC35</t>
+    <t>TC37</t>
   </si>
   <si>
     <t>Upload oversized file</t>
@@ -502,7 +558,7 @@
     <t>Reject with error message</t>
   </si>
   <si>
-    <t>TC36</t>
+    <t>TC38</t>
   </si>
   <si>
     <t>Invalid characters</t>
@@ -514,7 +570,7 @@
     <t>Text displays correctly</t>
   </si>
   <si>
-    <t>TC37</t>
+    <t>TC39</t>
   </si>
   <si>
     <t>Slow network</t>
@@ -526,7 +582,7 @@
     <t>Video loads or shows buffering</t>
   </si>
   <si>
-    <t>TC38</t>
+    <t>TC40</t>
   </si>
   <si>
     <t>Multiple sessions</t>
@@ -538,7 +594,7 @@
     <t>Actions sync correctly</t>
   </si>
   <si>
-    <t>TC39</t>
+    <t>TC41</t>
   </si>
   <si>
     <t>Unsupported browser</t>
@@ -969,10 +1025,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1166,13 +1222,15 @@
       <c r="B12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="1"/>
+      <c r="E12" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" ht="66" customHeight="1">
@@ -1182,13 +1240,15 @@
       <c r="B13" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>45</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="1"/>
+      <c r="E13" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" ht="66" customHeight="1">
@@ -1198,45 +1258,51 @@
       <c r="B14" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" ht="66" customHeight="1">
+    <row r="15" spans="1:6" ht="94.5" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E15" s="1"/>
+      <c r="E15" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" ht="66" customHeight="1">
+    <row r="16" spans="1:6" ht="54" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E16" s="1"/>
+      <c r="E16" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" ht="66" customHeight="1">
@@ -1246,13 +1312,15 @@
       <c r="B17" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E17" s="1"/>
+      <c r="E17" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" ht="66" customHeight="1">
@@ -1262,70 +1330,78 @@
       <c r="B18" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E18" s="1"/>
+      <c r="E18" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" ht="66" customHeight="1">
+    <row r="19" spans="1:6" ht="92.25" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E19" s="1"/>
+      <c r="E19" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" ht="28.5" customHeight="1">
-      <c r="A20" s="10" t="s">
+    <row r="20" spans="1:6" ht="81.75" customHeight="1">
+      <c r="A20" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="B20" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" ht="51" customHeight="1">
+    <row r="21" spans="1:6" ht="81" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E21" s="1"/>
+        <v>76</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" ht="51" customHeight="1">
-      <c r="A22" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D22" s="1" t="s">
+    <row r="22" spans="1:6" ht="28.5" customHeight="1">
+      <c r="A22" s="10" t="s">
         <v>79</v>
       </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
@@ -1393,46 +1469,46 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" ht="48.75" customHeight="1">
-      <c r="A27" s="11" t="s">
+    <row r="27" spans="1:6" ht="51" customHeight="1">
+      <c r="A27" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B27" s="11"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
+      <c r="B27" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" ht="63" customHeight="1">
+    <row r="28" spans="1:6" ht="51" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6" ht="63" customHeight="1">
-      <c r="A29" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D29" s="1" t="s">
+    <row r="29" spans="1:6" ht="48.75" customHeight="1">
+      <c r="A29" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="E29" s="1"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" ht="63" customHeight="1">
@@ -1531,185 +1607,217 @@
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="1:6" ht="42" customHeight="1">
-      <c r="A36" s="11" t="s">
+    <row r="36" spans="1:6" ht="63" customHeight="1">
+      <c r="A36" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B36" s="11"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
+      <c r="B36" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E36" s="1"/>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="1:6" ht="56.25" customHeight="1">
+    <row r="37" spans="1:6" ht="63" customHeight="1">
       <c r="A37" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="1:6" ht="56.25" customHeight="1">
-      <c r="A38" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E38" s="1"/>
+    <row r="38" spans="1:6" ht="42" customHeight="1">
+      <c r="A38" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B38" s="11"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
       <c r="F38" s="1"/>
     </row>
     <row r="39" spans="1:6" ht="56.25" customHeight="1">
       <c r="A39" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>73</v>
+        <v>140</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
     </row>
     <row r="40" spans="1:6" ht="56.25" customHeight="1">
       <c r="A40" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>70</v>
+        <v>145</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="1:6" ht="56.25" customHeight="1">
       <c r="A41" s="1" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>145</v>
+        <v>81</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="1:6" ht="29.25" customHeight="1">
-      <c r="A42" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="B42" s="11"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
+    <row r="42" spans="1:6" ht="56.25" customHeight="1">
+      <c r="A42" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E42" s="1"/>
       <c r="F42" s="1"/>
     </row>
-    <row r="43" spans="1:6" ht="59.25" customHeight="1">
+    <row r="43" spans="1:6" ht="56.25" customHeight="1">
       <c r="A43" s="1" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
     </row>
-    <row r="44" spans="1:6" ht="59.25" customHeight="1">
-      <c r="A44" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E44" s="1"/>
+    <row r="44" spans="1:6" ht="29.25" customHeight="1">
+      <c r="A44" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="B44" s="11"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
       <c r="F44" s="1"/>
     </row>
     <row r="45" spans="1:6" ht="59.25" customHeight="1">
       <c r="A45" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
     </row>
     <row r="46" spans="1:6" ht="59.25" customHeight="1">
       <c r="A46" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
     </row>
     <row r="47" spans="1:6" ht="59.25" customHeight="1">
       <c r="A47" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
+    </row>
+    <row r="48" spans="1:6" ht="59.25" customHeight="1">
+      <c r="A48" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+    </row>
+    <row r="49" spans="1:6" ht="59.25" customHeight="1">
+      <c r="A49" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated the rest of the YouTube test cases
</commit_message>
<xml_diff>
--- a/Youtube_Manual_Testing.xlsx
+++ b/Youtube_Manual_Testing.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29301"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29303"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="198" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{516EAA65-10BF-457A-A4EE-89DC1F55D552}"/>
+  <xr:revisionPtr revIDLastSave="390" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CBD08B7A-F1C2-49E2-82D4-F3027ADC05D1}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="179">
   <si>
     <t>Kevin Garry
 9/9/2025</t>
@@ -173,7 +173,7 @@
 2. Click the like button</t>
   </si>
   <si>
-    <t>Like count increases properly.</t>
+    <t>Like button turn into Unlike button. Like count increases properly.</t>
   </si>
   <si>
     <t>TC09</t>
@@ -186,7 +186,7 @@
 2. Click the dislike button</t>
   </si>
   <si>
-    <t>Dislike count increases correctly.</t>
+    <t>Dislike button becomes white. Dislike count increases correctly.</t>
   </si>
   <si>
     <t>TC10</t>
@@ -315,73 +315,86 @@
     <t>TC18</t>
   </si>
   <si>
-    <t>Search video</t>
-  </si>
-  <si>
-    <t>Enter keyword</t>
-  </si>
-  <si>
-    <t>Relevant results displayed</t>
+    <t>User enters valid text to search for a video.</t>
+  </si>
+  <si>
+    <t>1. Click on the search bar
+2. Enter valid text
+3. Click the search button</t>
+  </si>
+  <si>
+    <t>Shows relevant results to what the user put in the search bar.</t>
   </si>
   <si>
     <t>TC19</t>
   </si>
   <si>
-    <t>Search filters</t>
-  </si>
-  <si>
-    <t>Apply filters (date, duration)</t>
-  </si>
-  <si>
-    <t>Results update correctly</t>
+    <t>User searches for a video using the over 20 minute filter.</t>
+  </si>
+  <si>
+    <t>1. Click on the search bar
+2. Enter valid text
+3. Click the search button
+4. Click the filters button
+5. Select Over 20 minutes</t>
+  </si>
+  <si>
+    <t>Shows relevant results to what the user put in the search bar. Results are filtered to videos that are longer than 20 minutes.</t>
   </si>
   <si>
     <t>TC20</t>
   </si>
   <si>
-    <t>Trending tab</t>
-  </si>
-  <si>
-    <t>Click trending</t>
-  </si>
-  <si>
-    <t>Trending videos displayed</t>
+    <t>User searches for trending gaming videos.</t>
+  </si>
+  <si>
+    <t>1. Click the Gaming button in the Explore menu
+2. Search for the Trending videos category
+3. Click View all</t>
+  </si>
+  <si>
+    <t>Trending gaming videos are displayed to the user.</t>
   </si>
   <si>
     <t>TC21</t>
   </si>
   <si>
-    <t>Category navigation</t>
-  </si>
-  <si>
-    <t>Click music, gaming, news</t>
-  </si>
-  <si>
-    <t>Videos update correctly</t>
+    <t>User searches through multiple categories.</t>
+  </si>
+  <si>
+    <t>1. Click the Music button in the Explore menu
+2. Click the Gaming button in the Explore menu
+3. Click the News button in the Explore menu</t>
+  </si>
+  <si>
+    <t>Videos displayed are updated properly depending on which category the user is selecting.</t>
   </si>
   <si>
     <t>TC22</t>
   </si>
   <si>
-    <t>Video suggestions</t>
-  </si>
-  <si>
-    <t>Play video</t>
-  </si>
-  <si>
-    <t>Related videos suggested</t>
+    <t>User plays video to completion and suggested videos appear.</t>
+  </si>
+  <si>
+    <t>1. Navigate to a video
+2. Finish the video
+3. Make sure auto play is disabled</t>
+  </si>
+  <si>
+    <t>Suggested videos display when the video is finished.</t>
   </si>
   <si>
     <t>TC23</t>
   </si>
   <si>
-    <t>Pagination/load more</t>
-  </si>
-  <si>
-    <t>Scroll or click next</t>
-  </si>
-  <si>
-    <t>More videos load</t>
+    <t>User scrolls down while in the video display page to load more videos on the right side of the screen.</t>
+  </si>
+  <si>
+    <t>1. Navigate to a video
+2. Scroll down on the video display page</t>
+  </si>
+  <si>
+    <t>More videos are loaded as the user scrolls down.</t>
   </si>
   <si>
     <t>Upload &amp; Account Features</t>
@@ -390,97 +403,136 @@
     <t>TC24</t>
   </si>
   <si>
-    <t>Upload video</t>
-  </si>
-  <si>
-    <t>Upload valid file</t>
-  </si>
-  <si>
-    <t>Video processes &amp; publishes</t>
+    <t>User uploads a video to their YouTube channel.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Login with valid credentials
+2. Click the profile icon in the top right
+3. Click YouTube Studio
+4. Click Upload videos
+5. Select valid file
+6. Edit description and click next
+7. Edit video elements and click next
+8. Click next on the Checks tab
+9. Select visibility options and click save
+</t>
+  </si>
+  <si>
+    <t>Video uploads properly and shows up on the Channel content page.</t>
   </si>
   <si>
     <t>TC25</t>
   </si>
   <si>
-    <t>Edit video details</t>
-  </si>
-  <si>
-    <t>Change title/description</t>
-  </si>
-  <si>
-    <t>Changes saved correctly</t>
+    <t>User edits the video details on a video that have uploaded.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Login with valid credentials
+2. Click the profile icon in the top right
+3. Click YouTube Studio
+4. Click Upload videos
+5. Select valid file
+6. Edit description and click next
+</t>
+  </si>
+  <si>
+    <t>Changes are saved and applied to the video upload.</t>
   </si>
   <si>
     <t>TC26</t>
   </si>
   <si>
-    <t>Private/Public</t>
-  </si>
-  <si>
-    <t>Set visibility</t>
-  </si>
-  <si>
-    <t>Video visibility updates</t>
+    <t>User changes the visibility settings on a video they upload.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Login with valid credentials
+2. Click the profile icon in the top right
+3. Click YouTube Studio
+4. Click Upload videos
+5. Select valid file
+6. Edit description and click next
+7. Edit video elements and click next
+</t>
+  </si>
+  <si>
+    <t>Video visibility is set and saved properly. Video shows correctly depending on which video setting is selected.</t>
   </si>
   <si>
     <t>TC27</t>
   </si>
   <si>
-    <t>Delete video</t>
-  </si>
-  <si>
-    <t>Delete uploaded video</t>
-  </si>
-  <si>
-    <t>Video removed from account</t>
+    <t>User deletes a video they have uploaded.</t>
+  </si>
+  <si>
+    <t>1. Login with valid credentials
+2. Click the profile icon in the top right
+3. Click YouTube Studio
+4. Click the Content button
+5. Select video user wishes to delete
+6. Click more actions
+7. Click Delete forever
+8. Click the checkbox to confirm deletion of video
+9. Click Delete forever button</t>
+  </si>
+  <si>
+    <t>Video is deleted properly. Video no longer shows up on the Channel content page.</t>
   </si>
   <si>
     <t>TC28</t>
   </si>
   <si>
-    <t>Video thumbnail</t>
-  </si>
-  <si>
-    <t>Change thumbnail</t>
-  </si>
-  <si>
-    <t>Thumbnail updates correctly</t>
+    <t>User changes the thumbnail on a previously uploaded video.</t>
+  </si>
+  <si>
+    <t>1. Login with valid credentials
+2. Click the profile icon in the top right
+3. Click YouTube Studio
+4. Click the Content button
+5. Select a previously uploaded video
+6. Click Upload file under the Thumbnail header
+7. Select valid file</t>
+  </si>
+  <si>
+    <t>Thumbnail is video is updated in Channel content page and on the user's dashboard.</t>
   </si>
   <si>
     <t>TC29</t>
   </si>
   <si>
-    <t>View history</t>
-  </si>
-  <si>
-    <t>Play videos</t>
-  </si>
-  <si>
-    <t>History records played videos</t>
+    <t>User looks at previously viewed videos through the history page.</t>
+  </si>
+  <si>
+    <t>1. Login with valid credentials
+2. Click the History button</t>
+  </si>
+  <si>
+    <t>History tab correctly records and displays previously viewed videos.</t>
   </si>
   <si>
     <t>TC30</t>
   </si>
   <si>
-    <t>Liked videos</t>
-  </si>
-  <si>
-    <t>Like video</t>
-  </si>
-  <si>
-    <t>Appears in liked list</t>
+    <t>User looks at videos they have pressed the like button for.</t>
+  </si>
+  <si>
+    <t>1. Login with valid credentials
+2. Click the Liked videos button</t>
+  </si>
+  <si>
+    <t>All videos liked by the user are displayed properly.</t>
   </si>
   <si>
     <t>TC31</t>
   </si>
   <si>
-    <t>Watch later</t>
-  </si>
-  <si>
-    <t>Add video</t>
-  </si>
-  <si>
-    <t>Appears in “Watch Later”</t>
+    <t>User views videos they have saved to their watch latyer playlist.</t>
+  </si>
+  <si>
+    <t>1. Login with valid credentials
+2. Click the Watch later button</t>
+  </si>
+  <si>
+    <t>All videos previously added to watch later playlist are displayed properly.</t>
   </si>
   <si>
     <t>Mobile / Responsiveness</t>
@@ -489,58 +541,64 @@
     <t>TC32</t>
   </si>
   <si>
-    <t>Mobile playback</t>
-  </si>
-  <si>
-    <t>Play video on mobile</t>
-  </si>
-  <si>
-    <t>Plays correctly with responsive layout</t>
+    <t>User plays a video on an Iphone.</t>
+  </si>
+  <si>
+    <t>1. Navigate to a video
+2. Tap the play button</t>
+  </si>
+  <si>
+    <t>Video displays in the correct format and plays properly.</t>
   </si>
   <si>
     <t>TC33</t>
   </si>
   <si>
-    <t>Mobile commenting</t>
-  </si>
-  <si>
-    <t>Add comment</t>
-  </si>
-  <si>
-    <t>Appears properly</t>
+    <t>User comments on a video using an Iphone.</t>
+  </si>
+  <si>
+    <t>1. Navigate to a video
+2. Tap add a comment
+3. Enter valid text
+4. Tap the Comment button</t>
   </si>
   <si>
     <t>TC34</t>
   </si>
   <si>
-    <t>Mobile search</t>
-  </si>
-  <si>
-    <t>Results display correctly</t>
+    <t>User enters valid text to search for a video on an Iphone.</t>
+  </si>
+  <si>
+    <t>1. Tap on the search bar
+2. Enter valid text
+3. Tap the search button</t>
   </si>
   <si>
     <t>TC35</t>
   </si>
   <si>
-    <t>Mobile notifications</t>
-  </si>
-  <si>
-    <t>Subscribe → new video</t>
-  </si>
-  <si>
-    <t>Notification appears</t>
+    <t>User gets a notification on an Iphone that a channel they are subscribed to has uploaded a video.</t>
+  </si>
+  <si>
+    <t>1. Navigate to another user's channel
+2. Tap the subscribe button
+3. Tap the subscribed button
+4. Select All
+5. Wait for that User to upload a video</t>
   </si>
   <si>
     <t>TC36</t>
   </si>
   <si>
-    <t>Mobile fullscreen</t>
-  </si>
-  <si>
-    <t>Toggle fullscreen</t>
-  </si>
-  <si>
-    <t>Video fills screen correctly</t>
+    <t>User watches a video in fullscreen mode.</t>
+  </si>
+  <si>
+    <t>1. Navigate to a video
+2. Tap the full screen button or hold phone horizontally
+3. Tap the play button</t>
+  </si>
+  <si>
+    <t>Video is displayed properly in full screen format.</t>
   </si>
   <si>
     <t>Edge Cases / Exploratory</t>
@@ -549,61 +607,82 @@
     <t>TC37</t>
   </si>
   <si>
-    <t>Upload oversized file</t>
-  </si>
-  <si>
-    <t>Upload &gt; max size</t>
-  </si>
-  <si>
-    <t>Reject with error message</t>
+    <t>User uploads a video using a file that is too large.</t>
+  </si>
+  <si>
+    <t>1. Login with valid credentials
+2. Click the profile icon in the top right
+3. Click YouTube Studio
+4. Click Upload videos
+5. Select a file that is greater than 256 GB</t>
+  </si>
+  <si>
+    <t>User gets rejected and and receives an error message "File is too large.".</t>
   </si>
   <si>
     <t>TC38</t>
   </si>
   <si>
-    <t>Invalid characters</t>
-  </si>
-  <si>
-    <t>Add comment with emojis/special chars</t>
-  </si>
-  <si>
-    <t>Text displays correctly</t>
+    <t>User leaves a comment on a video using special characters.</t>
+  </si>
+  <si>
+    <t>1. Navigate to a video
+2. Click add a comment
+3. Enter valid text with emojis/special characters
+4. Click the Comment button</t>
+  </si>
+  <si>
+    <t>Comment is displayed under the video in the comments section and displayed properly.</t>
   </si>
   <si>
     <t>TC39</t>
   </si>
   <si>
-    <t>Slow network</t>
-  </si>
-  <si>
-    <t>Play video on slow connection</t>
-  </si>
-  <si>
-    <t>Video loads or shows buffering</t>
+    <t>User plays a video while having poor internet connection.</t>
+  </si>
+  <si>
+    <t>Video automatically tries to load using lower quality settings. Video buffers and continue trying to load if connection is poor enough.</t>
   </si>
   <si>
     <t>TC40</t>
   </si>
   <si>
-    <t>Multiple sessions</t>
-  </si>
-  <si>
-    <t>Login from 2 devices</t>
-  </si>
-  <si>
-    <t>Actions sync correctly</t>
-  </si>
-  <si>
-    <t>TC41</t>
-  </si>
-  <si>
-    <t>Unsupported browser</t>
-  </si>
-  <si>
-    <t>Open site in legacy browser</t>
-  </si>
-  <si>
-    <t>Site degrades gracefully or shows warning</t>
+    <t>User logs into YouTube on two different devices.</t>
+  </si>
+  <si>
+    <t>1. Login with valid credentials on a computer using a web browser
+2. Login with same valid credentials on the YouTube mobile app
+3. Select a video on the web browser
+4. Click the play button
+5. Select a different video on the mobile app
+6. Tap the play button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Each device functions properly and actions are synced up to the users account from both instances. </t>
+  </si>
+  <si>
+    <t>Bug ID</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Steps to Reproduce</t>
+  </si>
+  <si>
+    <t>Actual Result</t>
+  </si>
+  <si>
+    <t>Severity</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Screenshot</t>
+  </si>
+  <si>
+    <t>No bugs found.</t>
   </si>
 </sst>
 </file>
@@ -1028,7 +1107,7 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1079,7 +1158,7 @@
       <c r="E3" s="8"/>
       <c r="F3" s="9"/>
     </row>
-    <row r="4" spans="1:6" ht="38.25" customHeight="1">
+    <row r="4" spans="1:6" ht="53.25" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1097,7 +1176,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" ht="69" customHeight="1">
+    <row r="5" spans="1:6" ht="84.75" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1225,7 +1304,7 @@
       <c r="C12" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="2" t="s">
         <v>42</v>
       </c>
       <c r="E12" s="1" t="s">
@@ -1243,7 +1322,7 @@
       <c r="C13" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="2" t="s">
         <v>46</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -1412,61 +1491,69 @@
       <c r="B23" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E23" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" ht="51" customHeight="1">
+    <row r="24" spans="1:6" ht="81.75" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="E24" s="1"/>
+      <c r="E24" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" ht="51" customHeight="1">
+    <row r="25" spans="1:6" ht="84.75" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E25" s="1"/>
+      <c r="E25" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" ht="51" customHeight="1">
+    <row r="26" spans="1:6" ht="95.25" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E26" s="1"/>
+      <c r="E26" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" ht="51" customHeight="1">
@@ -1476,29 +1563,33 @@
       <c r="B27" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E27" s="1"/>
+      <c r="E27" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" ht="51" customHeight="1">
+    <row r="28" spans="1:6" ht="72.75" customHeight="1">
       <c r="A28" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="E28" s="1"/>
+      <c r="E28" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6" ht="48.75" customHeight="1">
@@ -1511,84 +1602,94 @@
       <c r="E29" s="10"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" ht="63" customHeight="1">
+    <row r="30" spans="1:6" ht="140.25" customHeight="1">
       <c r="A30" s="1" t="s">
         <v>105</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="E30" s="1"/>
+      <c r="E30" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6" ht="63" customHeight="1">
+    <row r="31" spans="1:6" ht="100.5" customHeight="1">
       <c r="A31" s="1" t="s">
         <v>109</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E31" s="1"/>
+      <c r="E31" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6" ht="63" customHeight="1">
+    <row r="32" spans="1:6" ht="113.25" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>113</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="E32" s="1"/>
+      <c r="E32" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" ht="63" customHeight="1">
+    <row r="33" spans="1:6" ht="157.5" customHeight="1">
       <c r="A33" s="1" t="s">
         <v>117</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E33" s="1"/>
+      <c r="E33" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="1:6" ht="63" customHeight="1">
+    <row r="34" spans="1:6" ht="132.75" customHeight="1">
       <c r="A34" s="1" t="s">
         <v>121</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E34" s="1"/>
+      <c r="E34" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F34" s="1"/>
     </row>
     <row r="35" spans="1:6" ht="63" customHeight="1">
@@ -1598,13 +1699,15 @@
       <c r="B35" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E35" s="1"/>
+      <c r="E35" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F35" s="1"/>
     </row>
     <row r="36" spans="1:6" ht="63" customHeight="1">
@@ -1614,13 +1717,15 @@
       <c r="B36" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E36" s="1"/>
+      <c r="E36" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F36" s="1"/>
     </row>
     <row r="37" spans="1:6" ht="63" customHeight="1">
@@ -1630,13 +1735,15 @@
       <c r="B37" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D37" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="E37" s="1"/>
+      <c r="E37" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F37" s="1"/>
     </row>
     <row r="38" spans="1:6" ht="42" customHeight="1">
@@ -1656,82 +1763,92 @@
       <c r="B39" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D39" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="E39" s="1"/>
+      <c r="E39" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="1:6" ht="56.25" customHeight="1">
+    <row r="40" spans="1:6" ht="67.5" customHeight="1">
       <c r="A40" s="1" t="s">
         <v>142</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E40" s="1"/>
+      <c r="D40" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="1:6" ht="56.25" customHeight="1">
       <c r="A41" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D41" s="1" t="s">
+      <c r="D41" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41" s="1"/>
+    </row>
+    <row r="42" spans="1:6" ht="84" customHeight="1">
+      <c r="A42" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-    </row>
-    <row r="42" spans="1:6" ht="56.25" customHeight="1">
-      <c r="A42" s="1" t="s">
+      <c r="B42" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="C42" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="D42" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42" s="1"/>
+    </row>
+    <row r="43" spans="1:6" ht="70.5" customHeight="1">
+      <c r="A43" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="B43" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-    </row>
-    <row r="43" spans="1:6" ht="56.25" customHeight="1">
-      <c r="A43" s="1" t="s">
+      <c r="C43" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E43" s="1"/>
+      <c r="E43" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F43" s="1"/>
     </row>
     <row r="44" spans="1:6" ht="29.25" customHeight="1">
       <c r="A44" s="10" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B44" s="11"/>
       <c r="C44" s="10"/>
@@ -1739,83 +1856,83 @@
       <c r="E44" s="10"/>
       <c r="F44" s="1"/>
     </row>
-    <row r="45" spans="1:6" ht="59.25" customHeight="1">
+    <row r="45" spans="1:6" ht="84" customHeight="1">
       <c r="A45" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="D45" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="E45" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F45" s="1"/>
+    </row>
+    <row r="46" spans="1:6" ht="81.75" customHeight="1">
+      <c r="A46" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="B46" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-    </row>
-    <row r="46" spans="1:6" ht="59.25" customHeight="1">
-      <c r="A46" s="1" t="s">
+      <c r="C46" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="D46" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="E46" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F46" s="1"/>
+    </row>
+    <row r="47" spans="1:6" ht="68.25" customHeight="1">
+      <c r="A47" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="B47" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-    </row>
-    <row r="47" spans="1:6" ht="59.25" customHeight="1">
-      <c r="A47" s="1" t="s">
+      <c r="C47" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="E47" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F47" s="1"/>
+    </row>
+    <row r="48" spans="1:6" ht="139.5" customHeight="1">
+      <c r="A48" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="B48" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="C48" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-    </row>
-    <row r="48" spans="1:6" ht="59.25" customHeight="1">
-      <c r="A48" s="1" t="s">
+      <c r="D48" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E48" s="1"/>
+      <c r="E48" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F48" s="1"/>
     </row>
-    <row r="49" spans="1:6" ht="59.25" customHeight="1">
-      <c r="A49" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>177</v>
-      </c>
+    <row r="49" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A49" s="1"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
     </row>
@@ -1826,12 +1943,56 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E4F67D3-3FB3-47EC-8E17-372FDE7A2797}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="8" width="20.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="44.25" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>